<commit_message>
[1.linear regression] last fix
</commit_message>
<xml_diff>
--- a/1.linear regression/houses.xlsx
+++ b/1.linear regression/houses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3ecfb898a1419d2/Desktop/ML/MasterML/1.linear regression/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B24B54B5-0DC3-4DF2-A5B5-E7151913AFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{51BEF4D1-AEB3-4C4D-B8E2-CDA32F4D1292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="houses" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="houses" localSheetId="0">houses!$A$1:$D$24</definedName>
+    <definedName name="houses" localSheetId="0">houses!$A$1:$D$32</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -909,10 +909,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1054,10 +1054,10 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>2000</v>
+        <v>2100</v>
       </c>
       <c r="D10">
-        <v>225000</v>
+        <v>230000</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1068,10 +1068,10 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <v>1750</v>
+        <v>2000</v>
       </c>
       <c r="D11">
-        <v>210000</v>
+        <v>225000</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1082,10 +1082,10 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>1700</v>
+        <v>1750</v>
       </c>
       <c r="D12">
-        <v>200000</v>
+        <v>210000</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1096,10 +1096,10 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <v>1650</v>
+        <v>1850</v>
       </c>
       <c r="D13">
-        <v>195000</v>
+        <v>225000</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1110,10 +1110,10 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>1900</v>
+        <v>1800</v>
       </c>
       <c r="D14">
-        <v>240000</v>
+        <v>210000</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1124,10 +1124,10 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <v>1300</v>
+        <v>1700</v>
       </c>
       <c r="D15">
-        <v>160000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1138,10 +1138,10 @@
         <v>15</v>
       </c>
       <c r="C16">
-        <v>2500</v>
+        <v>1650</v>
       </c>
       <c r="D16">
-        <v>325000</v>
+        <v>195000</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1152,10 +1152,10 @@
         <v>16</v>
       </c>
       <c r="C17">
-        <v>1400</v>
+        <v>1900</v>
       </c>
       <c r="D17">
-        <v>170000</v>
+        <v>240000</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1166,10 +1166,10 @@
         <v>17</v>
       </c>
       <c r="C18">
-        <v>2050</v>
+        <v>1300</v>
       </c>
       <c r="D18">
-        <v>235000</v>
+        <v>160000</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1180,10 +1180,10 @@
         <v>18</v>
       </c>
       <c r="C19">
-        <v>2250</v>
+        <v>2500</v>
       </c>
       <c r="D19">
-        <v>275000</v>
+        <v>325000</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1194,10 +1194,10 @@
         <v>19</v>
       </c>
       <c r="C20">
-        <v>1600</v>
+        <v>1500</v>
       </c>
       <c r="D20">
-        <v>190000</v>
+        <v>155000</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1208,10 +1208,10 @@
         <v>20</v>
       </c>
       <c r="C21">
-        <v>1950</v>
+        <v>1400</v>
       </c>
       <c r="D21">
-        <v>230000</v>
+        <v>170000</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1222,10 +1222,10 @@
         <v>21</v>
       </c>
       <c r="C22">
-        <v>2200</v>
+        <v>2000</v>
       </c>
       <c r="D22">
-        <v>300000</v>
+        <v>220000</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1236,10 +1236,10 @@
         <v>22</v>
       </c>
       <c r="C23">
-        <v>1800</v>
+        <v>2135</v>
       </c>
       <c r="D23">
-        <v>250000</v>
+        <v>245000</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1250,9 +1250,121 @@
         <v>23</v>
       </c>
       <c r="C24">
+        <v>2050</v>
+      </c>
+      <c r="D24">
+        <v>235000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>2250</v>
+      </c>
+      <c r="D25">
+        <v>275000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>1600</v>
+      </c>
+      <c r="D26">
+        <v>190000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>1950</v>
+      </c>
+      <c r="D27">
+        <v>230000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>2500</v>
+      </c>
+      <c r="D28">
+        <v>340000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>2200</v>
+      </c>
+      <c r="D29">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>1800</v>
+      </c>
+      <c r="D30">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>1350</v>
+      </c>
+      <c r="D31">
+        <v>145000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32">
         <v>1250</v>
       </c>
-      <c r="D24">
+      <c r="D32">
         <v>145000</v>
       </c>
     </row>

</xml_diff>